<commit_message>
add touchGFX DEMO GUI
</commit_message>
<xml_diff>
--- a/libraries/touchgfx_lib/TouchGFX/assets/texts/texts.xlsx
+++ b/libraries/touchgfx_lib/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="76">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -128,49 +128,121 @@
     <t xml:space="preserve">GB</t>
   </si>
   <si>
-    <t xml:space="preserve">Widget Wildcard Characters</t>
-  </si>
-  <si>
     <t xml:space="preserve">Default</t>
   </si>
   <si>
-    <t xml:space="preserve">verdana.ttf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotoSans-Regular.ttf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-., 0123456789</t>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;val&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scroll Wheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrollWhellTxt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrollWhellTxt_Highlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headline_ScrollWheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button_ScrollWheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headline_ScrollList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button_ScrollList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scroll List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Regular.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Medium.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Black.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">headline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title_ScrollList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title_ScrollWheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selected icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selected value</t>
   </si>
   <si>
     <t xml:space="preserve">SingleUseId1</t>
   </si>
   <si>
-    <t xml:space="preserve">Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTR</t>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
+    <t xml:space="preserve">Sle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crollWhellTxt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScrollWhellTxt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScrollWhellTxt_Highlight</t>
   </si>
 </sst>
 </file>
@@ -271,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -438,15 +510,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -532,7 +595,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -568,8 +631,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -918,18 +979,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:I100" totalsRowShown="0" tableBorderDxfId="9">
   <sortState ref="B4:E6">
     <sortCondition descending="1" ref="B3:B65536"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="8">
     <tableColumn id="1" name="Typography Name"/>
     <tableColumn id="2" name="Font"/>
     <tableColumn id="3" name="Size"/>
     <tableColumn id="4" name="Bpp"/>
     <tableColumn id="5" name="Fallback Character"/>
     <tableColumn id="6" name="Wildcard Characters"/>
-    <tableColumn id="9" name="Widget Wildcard Characters"/>
     <tableColumn id="7" name="Wildcard Ranges"/>
     <tableColumn id="8" name="Ellipsis Character"/>
   </tableColumns>
@@ -938,7 +998,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="K4:O10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
     <tableColumn id="1" name="Column" dataDxfId="4"/>
     <tableColumn id="2" name="Description" dataDxfId="3"/>
@@ -1322,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P12"/>
+  <dimension ref="B1:O12"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1337,37 +1397,35 @@
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="0" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="0" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="0" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="0" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="0" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="0" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="0" customWidth="1"/>
-    <col min="13" max="13" width="84.7109375" style="0" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="0" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="0" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" style="0" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="0" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="0" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" style="0" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="0" customWidth="1"/>
+    <col min="12" max="12" width="84.7109375" style="0" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="0" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="0" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" style="0" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="129" hidden="1" customHeight="1">
+    <row r="1" spans="2:15" ht="129" hidden="1" customHeight="1">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:16" ht="39.95" customHeight="1" thickBot="1">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:15" ht="39.95" customHeight="1" thickBot="1">
+      <c r="B2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
@@ -1386,25 +1444,22 @@
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16">
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1413,137 +1468,191 @@
         <v>17</v>
       </c>
       <c r="G4"/>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
+      <c r="H4"/>
       <c r="I4"/>
-      <c r="J4"/>
-      <c r="L4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="L4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:15">
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
       <c r="I5"/>
-      <c r="J5"/>
-      <c r="L5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="M5" s="9">
+        <v>20</v>
+      </c>
       <c r="N5" s="9">
+        <v>36</v>
+      </c>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
         <v>20</v>
       </c>
-      <c r="O5" s="9">
-        <v>36</v>
-      </c>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="2:16">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
       <c r="I6"/>
-      <c r="J6"/>
-      <c r="L6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="M6" s="9">
+        <v>4</v>
+      </c>
       <c r="N6" s="9">
+        <v>8</v>
+      </c>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7">
+        <v>58</v>
+      </c>
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="O6" s="9">
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7"/>
+      <c r="K7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="I8"/>
+      <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="2:16">
-      <c r="L7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16">
-      <c r="L8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="8" t="s">
+      <c r="L8" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="M8" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="N8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="2:16">
-      <c r="L9" s="11" t="s">
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="K9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="L9" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="M9" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="N9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
-      <c r="L10" s="11" t="s">
+    <row r="10" spans="2:15">
+      <c r="K10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="13" t="s">
+      <c r="M10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="N10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="14"/>
-    </row>
-    <row r="11" spans="2:16">
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="2:16">
-      <c r="M12" s="16" t="s">
+      <c r="O10" s="14"/>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="L12" s="16" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1557,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F3"/>
+  <dimension ref="B1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1575,12 +1684,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="3.75" customHeight="1"/>
     <row r="2" spans="2:6" ht="33" customHeight="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="2:6" s="22" customFormat="1">
       <c r="B3" t="s">
@@ -1599,40 +1708,212 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-    </row>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6"/>
+    <row r="17" spans="2:6"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>